<commit_message>
done some small changes
</commit_message>
<xml_diff>
--- a/CallX/inputs/TestData.xlsx
+++ b/CallX/inputs/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="84">
   <si>
     <t>Category / Menu</t>
   </si>
@@ -689,7 +689,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,19 +743,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -764,10 +764,10 @@
         <v>12</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -775,19 +775,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -796,10 +796,10 @@
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -807,19 +807,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>13</v>
@@ -828,10 +828,10 @@
         <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J4" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -839,19 +839,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -860,10 +860,10 @@
         <v>10</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J5" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -871,19 +871,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>30</v>
@@ -892,10 +892,10 @@
         <v>31</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J6" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -903,19 +903,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>32</v>
@@ -924,10 +924,10 @@
         <v>12</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="J7" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,6 +1378,198 @@
       </c>
       <c r="J6" s="4">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="4">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3111,8 +3303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed sorting array method and added unique key index finder
</commit_message>
<xml_diff>
--- a/CallX/inputs/TestData.xlsx
+++ b/CallX/inputs/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="86">
   <si>
     <t>Category / Menu</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>publisher</t>
+  </si>
+  <si>
+    <t>campaign_name,publisher_name</t>
+  </si>
+  <si>
+    <t>offer_name,publisher_name</t>
   </si>
 </sst>
 </file>
@@ -362,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,9 +385,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,27 +693,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -731,10 +738,10 @@
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -743,31 +750,31 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="J2" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -775,31 +782,31 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="J3" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -807,127 +814,31 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="J4" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -941,7 +852,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,23 +1079,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J6"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1406,7 +1317,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J7" s="4">
         <v>16</v>
@@ -1438,7 +1349,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J8" s="4">
         <v>16</v>
@@ -1470,7 +1381,7 @@
         <v>10</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J9" s="4">
         <v>16</v>
@@ -1502,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J10" s="4">
         <v>16</v>
@@ -1534,7 +1445,7 @@
         <v>31</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J11" s="4">
         <v>16</v>
@@ -1566,7 +1477,7 @@
         <v>12</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J12" s="4">
         <v>16</v>
@@ -1765,227 +1676,227 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>53</v>
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="D19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="G19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>53</v>
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="4">
+      <c r="D20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="G20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>53</v>
+      <c r="A21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="D21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="4">
-        <v>19</v>
+      <c r="H21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>53</v>
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="D22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="4">
-        <v>19</v>
+      <c r="H22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J22" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>53</v>
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="4" t="s">
+      <c r="D23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="4">
-        <v>19</v>
+      <c r="I23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="D24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="H24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J24" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="4">
-        <v>15</v>
+      <c r="G25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" s="6">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1993,31 +1904,31 @@
         <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J26" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2025,31 +1936,31 @@
         <v>6</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J27" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2057,31 +1968,31 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J28" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2089,31 +2000,31 @@
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J29" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2121,31 +2032,31 @@
         <v>6</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J30" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2153,31 +2064,31 @@
         <v>6</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="J31" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2185,28 +2096,28 @@
         <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J32" s="4">
         <v>15</v>
@@ -2217,28 +2128,28 @@
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J33" s="4">
         <v>15</v>
@@ -2249,28 +2160,28 @@
         <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J34" s="4">
         <v>15</v>
@@ -2281,28 +2192,28 @@
         <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J35" s="4">
         <v>15</v>
@@ -2313,30 +2224,254 @@
         <v>6</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F43" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="H43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J43" s="4">
         <v>15</v>
       </c>
     </row>
@@ -2347,10 +2482,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,7 +2498,7 @@
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
     <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2401,19 +2536,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
@@ -2422,7 +2557,7 @@
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2">
         <v>16</v>
@@ -2433,19 +2568,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>10</v>
@@ -2454,7 +2589,7 @@
         <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2">
         <v>16</v>
@@ -2465,19 +2600,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -2486,7 +2621,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2">
         <v>16</v>
@@ -2497,19 +2632,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>9</v>
@@ -2518,7 +2653,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2">
         <v>16</v>
@@ -2529,19 +2664,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
@@ -2550,7 +2685,7 @@
         <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J6" s="2">
         <v>16</v>
@@ -2561,19 +2696,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -2582,7 +2717,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J7" s="2">
         <v>16</v>
@@ -2593,19 +2728,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -2614,425 +2749,105 @@
         <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J8" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="4" t="s">
+      <c r="G13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="4">
+      <c r="J13" s="4">
         <v>15</v>
       </c>
     </row>
@@ -3303,7 +3118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>